<commit_message>
Updated dev, will not build due to npm linking issues. Commit before switching to single image for three seperate runs
</commit_message>
<xml_diff>
--- a/Watch/Smarch BOM.xlsx
+++ b/Watch/Smarch BOM.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/Jarvis/Jarvis_Mark_7/Watch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061683D0-A08E-1643-BEF2-C30B6221D258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64145E6-6442-1E4C-977C-0C2FCA75143A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="15960" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1667,7 +1677,7 @@
   <dimension ref="A1:IV34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>